<commit_message>
Android and Firmware Update
Android update to fix Excel file data logging and recording
</commit_message>
<xml_diff>
--- a/Timesheets/2018-11-25.xlsx
+++ b/Timesheets/2018-11-25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdemolde\Documents\GitHub\Coleman-Nordic-Butterfly\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF600747-07A9-4549-B6AF-20919CF39DE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B35E8-17FC-43C0-93DB-C3A183D6FF28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,13 +123,13 @@
     <t>TODD COLEMAN</t>
   </si>
   <si>
-    <t>7/31/18</t>
-  </si>
-  <si>
     <t>UCSD CONTRACTING BI-WEEKLY TIME RECORD</t>
   </si>
   <si>
     <t>11/25/18-12/08/18</t>
+  </si>
+  <si>
+    <t>12/08/18</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -782,26 +782,19 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -821,10 +814,7 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -833,23 +823,20 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -865,7 +852,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -881,7 +868,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -897,7 +884,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -944,7 +931,7 @@
     <xf numFmtId="2" fontId="10" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -959,64 +946,80 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1025,19 +1028,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1047,11 +1050,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1060,51 +1063,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1590,7 +1548,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1634,7 +1592,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1659,10 +1617,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
@@ -1677,50 +1635,50 @@
   <sheetData>
     <row r="1" spans="1:18" ht="9" customHeight="1"/>
     <row r="2" spans="1:18" ht="23.1" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="112" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
+      <c r="B2" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
     </row>
     <row r="3" spans="1:18" ht="12.95" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
     </row>
     <row r="4" spans="1:18" ht="0.95" hidden="1" customHeight="1">
       <c r="B4" s="8"/>
@@ -1742,59 +1700,59 @@
       <c r="R4" s="10"/>
     </row>
     <row r="5" spans="1:18" ht="9" customHeight="1">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
       <c r="G5"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="15"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1">
-      <c r="B6" s="122" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
+      <c r="B6" s="93" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="93"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="108" t="s">
+      <c r="M6" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="109"/>
-      <c r="O6" s="109"/>
-      <c r="P6" s="109"/>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="109"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
     </row>
     <row r="7" spans="1:18" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="14"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="95" t="s">
@@ -1823,10 +1781,10 @@
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
-      <c r="R8" s="34"/>
+      <c r="R8" s="30"/>
     </row>
     <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="12"/>
@@ -1844,7 +1802,7 @@
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="35"/>
+      <c r="R9" s="31"/>
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="B10" s="106" t="s">
@@ -1853,46 +1811,46 @@
       <c r="C10" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="74" t="s">
+      <c r="H10" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="75" t="s">
+      <c r="I10" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="72" t="s">
+      <c r="J10" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="71" t="s">
+      <c r="K10" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="70" t="s">
+      <c r="L10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="71" t="s">
+      <c r="M10" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="70" t="s">
+      <c r="N10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="75" t="s">
+      <c r="O10" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="74" t="s">
+      <c r="P10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="73" t="s">
+      <c r="Q10" s="68" t="s">
         <v>8</v>
       </c>
       <c r="R10" s="7"/>
@@ -1900,49 +1858,49 @@
     <row r="11" spans="1:18" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="B11" s="107"/>
       <c r="C11" s="103"/>
-      <c r="D11" s="69">
+      <c r="D11" s="64">
         <v>41967</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="64">
         <v>41968</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="64">
         <v>41969</v>
       </c>
-      <c r="G11" s="69">
+      <c r="G11" s="64">
         <v>41970</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="64">
         <v>41971</v>
       </c>
-      <c r="I11" s="69">
+      <c r="I11" s="64">
         <v>41972</v>
       </c>
-      <c r="J11" s="69">
+      <c r="J11" s="64">
         <v>41973</v>
       </c>
-      <c r="K11" s="69">
+      <c r="K11" s="64">
         <v>41974</v>
       </c>
-      <c r="L11" s="69">
+      <c r="L11" s="64">
         <v>41975</v>
       </c>
-      <c r="M11" s="69">
+      <c r="M11" s="64">
         <v>41976</v>
       </c>
-      <c r="N11" s="69">
+      <c r="N11" s="64">
         <v>41977</v>
       </c>
-      <c r="O11" s="69">
+      <c r="O11" s="64">
         <v>41978</v>
       </c>
-      <c r="P11" s="69">
+      <c r="P11" s="64">
         <v>41979</v>
       </c>
-      <c r="Q11" s="69">
+      <c r="Q11" s="64">
         <v>41980</v>
       </c>
-      <c r="R11" s="59" t="s">
+      <c r="R11" s="54" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1950,535 +1908,501 @@
       <c r="B12" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="44">
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39">
         <v>3.5</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43">
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38">
         <v>2.5</v>
       </c>
-      <c r="O12" s="76">
+      <c r="O12" s="38">
         <v>3.5</v>
       </c>
-      <c r="P12" s="76">
+      <c r="P12" s="38">
         <v>2</v>
       </c>
-      <c r="Q12" s="44">
+      <c r="Q12" s="39">
         <v>3.5</v>
       </c>
-      <c r="R12" s="60">
+      <c r="R12" s="55">
         <f t="shared" ref="R12:R21" si="0">SUM(D12:Q12)</f>
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="33" customHeight="1" thickBot="1">
       <c r="B13" s="98"/>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="61">
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="33" customHeight="1">
       <c r="B14" s="97"/>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="78"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="60">
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="33" customHeight="1" thickBot="1">
       <c r="B15" s="98"/>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="62">
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="33" customHeight="1">
       <c r="B16" s="97"/>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="52"/>
-      <c r="R16" s="60">
+      <c r="D16" s="45"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="33" customHeight="1" thickBot="1">
+    <row r="17" spans="2:18" ht="33" customHeight="1" thickBot="1">
       <c r="B17" s="98"/>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="61">
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="33" customHeight="1">
+    <row r="18" spans="2:18" ht="33" customHeight="1">
       <c r="B18" s="97"/>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="78"/>
-      <c r="Q18" s="52"/>
-      <c r="R18" s="60">
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="33" customHeight="1" thickBot="1">
+    <row r="19" spans="2:18" ht="33" customHeight="1" thickBot="1">
       <c r="B19" s="98"/>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="61">
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:19" ht="33" customHeight="1">
+    <row r="20" spans="2:18" ht="33" customHeight="1">
       <c r="B20" s="104"/>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="78"/>
-      <c r="Q20" s="52"/>
-      <c r="R20" s="60">
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:19" ht="33" customHeight="1" thickBot="1">
+    <row r="21" spans="2:18" ht="33" customHeight="1" thickBot="1">
       <c r="B21" s="105"/>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="78"/>
-      <c r="P21" s="78"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="61">
+      <c r="D21" s="49"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="35.1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B22" s="116" t="s">
+    <row r="22" spans="2:18" ht="35.1" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B22" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="117"/>
-      <c r="D22" s="64">
+      <c r="C22" s="88"/>
+      <c r="D22" s="59">
         <f t="shared" ref="D22:Q22" si="1">SUM(D12:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="91">
+      <c r="E22" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F22" s="65">
+      <c r="F22" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="65">
+      <c r="G22" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="69">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="79">
+      <c r="I22" s="69">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J22" s="66">
+      <c r="J22" s="61">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="K22" s="67">
+      <c r="K22" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L22" s="65">
+      <c r="L22" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M22" s="65">
+      <c r="M22" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N22" s="65">
+      <c r="N22" s="60">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="O22" s="79">
+      <c r="O22" s="69">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="P22" s="79">
+      <c r="P22" s="69">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q22" s="68">
+      <c r="Q22" s="63">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="R22" s="63">
+      <c r="R22" s="58">
         <f>SUM(D22:Q22)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="29.1" customHeight="1">
-      <c r="E23" s="86" t="s">
+    <row r="23" spans="2:18" ht="29.1" customHeight="1">
+      <c r="E23" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="92" t="s">
-        <v>27</v>
+      <c r="F23" s="78" t="s">
+        <v>29</v>
       </c>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="2:19" ht="2.1" customHeight="1">
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="57" t="s">
+    <row r="24" spans="2:18" ht="2.1" customHeight="1">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
       <c r="H24"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="K24" s="33"/>
+      <c r="K24" s="29"/>
       <c r="L24"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="2:19" ht="15.95" customHeight="1">
-      <c r="B25" s="56" t="s">
+    <row r="25" spans="2:18" ht="15.95" customHeight="1">
+      <c r="B25" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="20"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="85"/>
-      <c r="R25" s="86"/>
-      <c r="S25" s="13"/>
-    </row>
-    <row r="26" spans="2:19" ht="12.95" customHeight="1">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="G26" s="16"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="51"/>
+    </row>
+    <row r="26" spans="2:18" ht="12.95" customHeight="1">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="H26"/>
       <c r="I26" s="99"/>
       <c r="J26" s="100"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="89"/>
-      <c r="O26" s="89"/>
-      <c r="P26" s="89"/>
-      <c r="Q26" s="90"/>
-      <c r="R26" s="86"/>
-      <c r="S26" s="13"/>
-    </row>
-    <row r="27" spans="2:19" ht="17.100000000000001" customHeight="1">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
+      <c r="P26" s="76"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="51"/>
+    </row>
+    <row r="27" spans="2:18" ht="17.100000000000001" customHeight="1">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="90"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-    </row>
-    <row r="28" spans="2:19" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B28" s="58" t="s">
+      <c r="G27" s="15"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
+      <c r="Q27" s="2"/>
+      <c r="R27"/>
+    </row>
+    <row r="28" spans="2:18" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="B28" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="94"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-      <c r="N28" s="88"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="88"/>
-      <c r="Q28" s="90"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-    </row>
-    <row r="29" spans="2:19" ht="21.95" customHeight="1" thickTop="1">
-      <c r="B29" s="18" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="83"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="2"/>
+      <c r="R28"/>
+    </row>
+    <row r="29" spans="2:18" ht="21.95" customHeight="1" thickTop="1">
+      <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="18"/>
+      <c r="C29" s="4"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="88"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
-      <c r="P29" s="88"/>
-      <c r="Q29" s="90"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-    </row>
-    <row r="30" spans="2:19" ht="21.95" customHeight="1">
+      <c r="I29" s="83"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="2"/>
+      <c r="R29"/>
+    </row>
+    <row r="30" spans="2:18" ht="21.95" customHeight="1">
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="13"/>
+      <c r="D30"/>
       <c r="E30"/>
-      <c r="F30" s="13"/>
+      <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="88"/>
-      <c r="N30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="90"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-    </row>
-    <row r="31" spans="2:19" ht="21.95" customHeight="1">
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="80"/>
-      <c r="M31" s="80"/>
-      <c r="N31" s="80"/>
-      <c r="O31" s="80"/>
-      <c r="P31" s="80"/>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="90"/>
-      <c r="S31" s="13"/>
-    </row>
-    <row r="32" spans="2:19" ht="21.95" customHeight="1">
+      <c r="H30"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="2"/>
+      <c r="R30"/>
+    </row>
+    <row r="31" spans="2:18" ht="21.95" customHeight="1">
+      <c r="D31"/>
+      <c r="G31"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+    </row>
+    <row r="32" spans="2:18" ht="21.95" customHeight="1">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
     </row>
     <row r="33" spans="2:7" ht="21.95" customHeight="1"/>
     <row r="34" spans="2:7" ht="21.95" customHeight="1"/>
     <row r="35" spans="2:7" ht="15" customHeight="1"/>
     <row r="36" spans="2:7" ht="15" customHeight="1"/>
     <row r="41" spans="2:7" ht="15.75">
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
-      <c r="G41" s="15"/>
+      <c r="G41" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B3:R3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="M7:R7"/>
@@ -2492,6 +2416,15 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>